<commit_message>
Concurrency test for multiple users
</commit_message>
<xml_diff>
--- a/Llama/Fusion_test_log.xlsx
+++ b/Llama/Fusion_test_log.xlsx
@@ -42,9 +42,10 @@
  Proven organizational and time management skills</t>
   </si>
   <si>
-    <t>Here is the tailored text:
-As a seasoned finance professional with 6+ years of experience in Financial Services, I possess a passion for grasping macro and micro aspects affecting corporate finances. My expertise lies in providing equity fund raising, debt syndication, M&amp;A, and investor relations services to over 50 companies across sectors including Healthcare, Life Sciences, Energy, Industrials, Consumer, and Technology.
-With a strong background in Investor Relations, Investment Banking, and Corporate Finance Advisory, I have honed competencies in business storytelling and problem-solving. These skills not only energize me emotionally but also enable me to thrive under pressure, manage deadlines, and navigate unexpected changes in expectations or requirements.</t>
+    <t>Here's a tailored version of the text that highlights your relevant experience and skills for the job description:
+As a seasoned finance professional with 6+ years of experience in Financial Services, I possess a unique blend of skills that enable me to excel in Global Project Management. My background in Investor Relations, Investment Banking, and Corporate Finance Advisory has equipped me with strong organizational and time management skills, allowing me to work efficiently under pressure and meet tight deadlines.
+Throughout my career, I have successfully delivered high-profile projects, including equity fund raising, debt syndication, M&amp;A, and investor relations services to over 50 companies across various sectors. This experience has honed my ability to manage competing priorities, adapt to unexpected changes, and maintain a strong sense of urgency in meeting project milestones.
+As someone who is passionate about business storytelling, I have developed a keen understanding of the macro and micro aspects that impact corporate finances. My problem-solving skills enable me to navigate complex financial scenarios and develop creative solutions that drive results. With my expertise in financial services and global project management, I am confident in my ability to take on new challenges and deliver exceptional outcomes.</t>
   </si>
 </sst>
 </file>

</xml_diff>